<commit_message>
Saving, AI, Documentation, etc.
</commit_message>
<xml_diff>
--- a/Documentation/Diagrams/Class_Diagrams.xlsx
+++ b/Documentation/Diagrams/Class_Diagrams.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28421"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
   <si>
     <t>Weapon</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>has_X...</t>
+  </si>
+  <si>
+    <t>Cross</t>
   </si>
 </sst>
 </file>
@@ -2188,8 +2191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2504,7 +2507,7 @@
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="8" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -3230,7 +3233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>

</xml_diff>